<commit_message>
CAMBIOS EN LAS VISTAS Y data
</commit_message>
<xml_diff>
--- a/data_ejemplo.xlsx
+++ b/data_ejemplo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\2sistema beneficios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\sistema_beneficios\SISTEMA_BENEFICIOS.02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23658861-4364-41DD-862D-A5A5D5B43AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540D9965-B89F-43F2-8B89-99C06063EEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="120" windowWidth="10230" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6009" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6021" uniqueCount="1168">
   <si>
     <t>Cedula</t>
   </si>
@@ -3491,6 +3491,39 @@
   </si>
   <si>
     <t>SANDOVAL FUENTES FERNANDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARVAJAL SALAS ANTHONY JESUS </t>
+  </si>
+  <si>
+    <t>BLANCO AGAMEZ LICETH AGNERYS</t>
+  </si>
+  <si>
+    <t>VILLEGAS TORREALBA AMERICO ALEXANDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALLENILLA JENNY MARYURI </t>
+  </si>
+  <si>
+    <t>DESPACHO DEL VICEMINISTRO (A)  DEL SISTEMA INTEGRADO DE INVESTIGACION PENAL</t>
+  </si>
+  <si>
+    <t>VICEMINISTERIO DEL SISTEMA INTEGRADO DE INVESTIGACION PENAL</t>
+  </si>
+  <si>
+    <t>DIRECCION DE ESTUDIOS NORMATIVOS Y DICTAMENES JURIDICOS</t>
+  </si>
+  <si>
+    <t>CONSULTORIA JURIDICA</t>
+  </si>
+  <si>
+    <t>DIRECCION GENERAL DE SEGURIDAD CIUDADANA</t>
+  </si>
+  <si>
+    <t>VICEMINISTERIO DE PREVENCION Y SEGURIDAD CIUDADANA Y CUADRANTES DE PAZ</t>
+  </si>
+  <si>
+    <t>DIRECCION GENERAL DEL SISTEMA DE INFORMACION DE INVESTIGACION PENAL</t>
   </si>
 </sst>
 </file>
@@ -3814,7 +3847,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -3929,6 +3962,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3974,8 +4022,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4331,10 +4382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1001"/>
+  <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
+      <selection activeCell="D1002" sqref="D1002"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33373,6 +33424,86 @@
         <v>9</v>
       </c>
     </row>
+    <row r="1002" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1002" s="1">
+        <v>16331027</v>
+      </c>
+      <c r="B1002" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C1002">
+        <v>1111</v>
+      </c>
+      <c r="D1002" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E1002" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F1002">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1003" s="1">
+        <v>13803804</v>
+      </c>
+      <c r="B1003" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C1003">
+        <v>1111</v>
+      </c>
+      <c r="D1003" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E1003" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F1003">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1004" s="1">
+        <v>9094750</v>
+      </c>
+      <c r="B1004" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C1004">
+        <v>1111</v>
+      </c>
+      <c r="D1004" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E1004" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F1004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1005" s="1">
+        <v>7956829</v>
+      </c>
+      <c r="B1005" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C1005">
+        <v>1111</v>
+      </c>
+      <c r="D1005" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E1005" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F1005">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>